<commit_message>
V5 Advanced Excel - Using Recommended Pivot Tables
</commit_message>
<xml_diff>
--- a/Synthpop CD Inventory.xlsx
+++ b/Synthpop CD Inventory.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Riki Documents\Coding\Excel Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54252D69-45E2-4EEA-97A6-0A2E47A198F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD25EB7-49C5-45F8-A324-2F38FCFFFC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="0" windowWidth="14580" windowHeight="15750" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14220" yWindow="0" windowWidth="14580" windowHeight="15750" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="13" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="43">
   <si>
     <t>Band</t>
   </si>
@@ -164,6 +166,9 @@
   </si>
   <si>
     <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Sum of Copies Sold</t>
   </si>
 </sst>
 </file>
@@ -359,6 +364,70 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Asus" refreshedDate="44622.864427083332" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="45" xr:uid="{C5D84EBA-0221-43FB-8A58-7B0D6B5D560B}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="Band" numFmtId="0">
+      <sharedItems count="12">
+        <s v="Blaqk Audio"/>
+        <s v="Covenant"/>
+        <s v="Depeche Mode"/>
+        <s v="Erasure"/>
+        <s v="Future Islands"/>
+        <s v="Hurts"/>
+        <s v="OMD"/>
+        <s v="The Frozen Autumn"/>
+        <s v="The Jellyrox"/>
+        <s v="The Killers"/>
+        <s v="Ulver"/>
+        <s v="Brandon Flowers"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Album" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Genre" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Synthpop"/>
+        <s v="Futurepop"/>
+        <s v="Electronic"/>
+        <s v="Pop"/>
+        <s v="Darkwave"/>
+        <s v="Rock"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Item Number" numFmtId="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="100235413287" maxValue="886513250804"/>
+    </cacheField>
+    <cacheField name="Price" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="5.77" maxValue="12.22"/>
+    </cacheField>
+    <cacheField name="Quarter" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="4">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Copies Sold" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="200"/>
+    </cacheField>
+    <cacheField name="Sales" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="27.599999999999998" maxValue="1841.4"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="45">
   <r>
@@ -814,8 +883,463 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="45">
+  <r>
+    <x v="0"/>
+    <s v="Material"/>
+    <x v="0"/>
+    <n v="658765770001"/>
+    <n v="9.1999999999999993"/>
+    <x v="0"/>
+    <n v="56"/>
+    <n v="515.19999999999993"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Material"/>
+    <x v="0"/>
+    <n v="658765770001"/>
+    <n v="9.1999999999999993"/>
+    <x v="1"/>
+    <n v="85"/>
+    <n v="781.99999999999989"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Material"/>
+    <x v="0"/>
+    <n v="658765770001"/>
+    <n v="9.1999999999999993"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="27.599999999999998"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Material"/>
+    <x v="0"/>
+    <n v="658765770001"/>
+    <n v="9.1999999999999993"/>
+    <x v="3"/>
+    <n v="45"/>
+    <n v="413.99999999999994"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="The Blinding Dark"/>
+    <x v="1"/>
+    <n v="658745982100"/>
+    <n v="11.3"/>
+    <x v="0"/>
+    <n v="20"/>
+    <n v="226"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="The Blinding Dark"/>
+    <x v="1"/>
+    <n v="658745982100"/>
+    <n v="11.3"/>
+    <x v="1"/>
+    <n v="75"/>
+    <n v="847.5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="The Blinding Dark"/>
+    <x v="1"/>
+    <n v="658745982100"/>
+    <n v="11.3"/>
+    <x v="2"/>
+    <n v="56"/>
+    <n v="632.80000000000007"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="The Blinding Dark"/>
+    <x v="1"/>
+    <n v="658745982100"/>
+    <n v="11.3"/>
+    <x v="3"/>
+    <n v="27"/>
+    <n v="305.10000000000002"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Spirit"/>
+    <x v="2"/>
+    <n v="101006587955"/>
+    <n v="5.77"/>
+    <x v="0"/>
+    <n v="189"/>
+    <n v="1090.53"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Spirit"/>
+    <x v="2"/>
+    <n v="101006587955"/>
+    <n v="5.77"/>
+    <x v="1"/>
+    <n v="150"/>
+    <n v="865.49999999999989"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Spirit"/>
+    <x v="2"/>
+    <n v="101006587955"/>
+    <n v="5.77"/>
+    <x v="2"/>
+    <n v="85"/>
+    <n v="490.45"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Spirit"/>
+    <x v="2"/>
+    <n v="101006587955"/>
+    <n v="5.77"/>
+    <x v="3"/>
+    <n v="192"/>
+    <n v="1107.8399999999999"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="World Be Gone"/>
+    <x v="0"/>
+    <n v="601100065879"/>
+    <n v="7.99"/>
+    <x v="0"/>
+    <n v="31"/>
+    <n v="247.69"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="World Be Gone"/>
+    <x v="0"/>
+    <n v="601100065879"/>
+    <n v="7.99"/>
+    <x v="1"/>
+    <n v="135"/>
+    <n v="1078.6500000000001"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="World Be Gone"/>
+    <x v="0"/>
+    <n v="601100065879"/>
+    <n v="7.99"/>
+    <x v="2"/>
+    <n v="75"/>
+    <n v="599.25"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="World Be Gone"/>
+    <x v="0"/>
+    <n v="601100065879"/>
+    <n v="7.99"/>
+    <x v="3"/>
+    <n v="76"/>
+    <n v="607.24"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="The Far Field"/>
+    <x v="0"/>
+    <n v="178012548711"/>
+    <n v="7.99"/>
+    <x v="0"/>
+    <n v="80"/>
+    <n v="639.20000000000005"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="The Far Field"/>
+    <x v="0"/>
+    <n v="178012548711"/>
+    <n v="7.99"/>
+    <x v="1"/>
+    <n v="74"/>
+    <n v="591.26"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="The Far Field"/>
+    <x v="0"/>
+    <n v="178012548711"/>
+    <n v="7.99"/>
+    <x v="2"/>
+    <n v="65"/>
+    <n v="519.35"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="The Far Field"/>
+    <x v="0"/>
+    <n v="178012548711"/>
+    <n v="7.99"/>
+    <x v="3"/>
+    <n v="89"/>
+    <n v="711.11"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Desire"/>
+    <x v="3"/>
+    <n v="351000587561"/>
+    <n v="11.1"/>
+    <x v="0"/>
+    <n v="15"/>
+    <n v="166.5"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Desire"/>
+    <x v="3"/>
+    <n v="351000587561"/>
+    <n v="11.1"/>
+    <x v="1"/>
+    <n v="85"/>
+    <n v="943.5"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Desire"/>
+    <x v="3"/>
+    <n v="351000587561"/>
+    <n v="11.1"/>
+    <x v="2"/>
+    <n v="32"/>
+    <n v="355.2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Desire"/>
+    <x v="3"/>
+    <n v="351000587561"/>
+    <n v="11.1"/>
+    <x v="3"/>
+    <n v="20"/>
+    <n v="222"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="The Punishment of Luxury"/>
+    <x v="0"/>
+    <n v="886513250804"/>
+    <n v="7.46"/>
+    <x v="0"/>
+    <n v="132"/>
+    <n v="984.72"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="The Punishment of Luxury"/>
+    <x v="0"/>
+    <n v="886513250804"/>
+    <n v="7.46"/>
+    <x v="1"/>
+    <n v="145"/>
+    <n v="1081.7"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="The Punishment of Luxury"/>
+    <x v="0"/>
+    <n v="886513250804"/>
+    <n v="7.46"/>
+    <x v="2"/>
+    <n v="73"/>
+    <n v="544.58000000000004"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="The Punishment of Luxury"/>
+    <x v="0"/>
+    <n v="886513250804"/>
+    <n v="7.46"/>
+    <x v="3"/>
+    <n v="46"/>
+    <n v="343.16"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="The Fellow Traveller"/>
+    <x v="4"/>
+    <n v="587005465891"/>
+    <n v="12.22"/>
+    <x v="0"/>
+    <n v="15"/>
+    <n v="183.3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="The Fellow Traveller"/>
+    <x v="4"/>
+    <n v="587005465891"/>
+    <n v="12.22"/>
+    <x v="1"/>
+    <n v="45"/>
+    <n v="549.9"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="The Fellow Traveller"/>
+    <x v="4"/>
+    <n v="587005465891"/>
+    <n v="12.22"/>
+    <x v="2"/>
+    <n v="12"/>
+    <n v="146.64000000000001"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="The Fellow Traveller"/>
+    <x v="4"/>
+    <n v="587005465891"/>
+    <n v="12.22"/>
+    <x v="3"/>
+    <n v="60"/>
+    <n v="733.2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Bang and Whimper"/>
+    <x v="0"/>
+    <n v="100235413287"/>
+    <n v="8"/>
+    <x v="0"/>
+    <n v="17"/>
+    <n v="136"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Bang and Whimper"/>
+    <x v="0"/>
+    <n v="100235413287"/>
+    <n v="8"/>
+    <x v="1"/>
+    <n v="8"/>
+    <n v="64"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Bang and Whimper"/>
+    <x v="0"/>
+    <n v="100235413287"/>
+    <n v="8"/>
+    <x v="2"/>
+    <n v="35"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Bang and Whimper"/>
+    <x v="0"/>
+    <n v="100235413287"/>
+    <n v="8"/>
+    <x v="3"/>
+    <n v="28"/>
+    <n v="224"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <s v="Wonderful Wonderful"/>
+    <x v="5"/>
+    <n v="175235411350"/>
+    <n v="11.88"/>
+    <x v="0"/>
+    <n v="155"/>
+    <n v="1841.4"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <s v="Wonderful Wonderful"/>
+    <x v="5"/>
+    <n v="175235411350"/>
+    <n v="11.88"/>
+    <x v="1"/>
+    <n v="85"/>
+    <n v="1009.8000000000001"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <s v="Wonderful Wonderful"/>
+    <x v="5"/>
+    <n v="175235411350"/>
+    <n v="11.88"/>
+    <x v="2"/>
+    <n v="155"/>
+    <n v="1841.4"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <s v="Wonderful Wonderful"/>
+    <x v="5"/>
+    <n v="175235411350"/>
+    <n v="11.88"/>
+    <x v="3"/>
+    <n v="155"/>
+    <n v="1841.4"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <s v="The Assassination of Julius Caesar"/>
+    <x v="0"/>
+    <n v="512548965412"/>
+    <n v="10.68"/>
+    <x v="0"/>
+    <n v="92"/>
+    <n v="982.56"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <s v="The Assassination of Julius Caesar"/>
+    <x v="0"/>
+    <n v="512548965412"/>
+    <n v="10.68"/>
+    <x v="1"/>
+    <n v="29"/>
+    <n v="309.71999999999997"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <s v="The Assassination of Julius Caesar"/>
+    <x v="0"/>
+    <n v="512548965412"/>
+    <n v="10.68"/>
+    <x v="2"/>
+    <n v="54"/>
+    <n v="576.72"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <s v="The Assassination of Julius Caesar"/>
+    <x v="0"/>
+    <n v="512548965412"/>
+    <n v="10.68"/>
+    <x v="3"/>
+    <n v="69"/>
+    <n v="736.92"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <s v="The Desired Effect"/>
+    <x v="3"/>
+    <n v="484020923023"/>
+    <n v="9"/>
+    <x v="0"/>
+    <n v="200"/>
+    <n v="1800"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A65C594-B8D5-4B26-9D39-475528B0ACCE}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A65C594-B8D5-4B26-9D39-475528B0ACCE}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -947,6 +1471,151 @@
   </pageFields>
   <dataFields count="1">
     <dataField name="Sum of Sales" fld="7" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{822E3C06-0993-4F81-BA26-C01756E59E48}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="0"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="5"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Copies Sold" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1313,7 +1982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5270E3EC-8B00-48B6-91BB-09688D966ECA}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1629,6 +2298,429 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D89570-4DD4-40BA-9B6C-3A4F4DC71E1C}">
+  <dimension ref="A3:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="8">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8">
+        <v>45</v>
+      </c>
+      <c r="D5" s="8">
+        <v>12</v>
+      </c>
+      <c r="E5" s="8">
+        <v>60</v>
+      </c>
+      <c r="F5" s="8">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="8">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8">
+        <v>45</v>
+      </c>
+      <c r="D6" s="8">
+        <v>12</v>
+      </c>
+      <c r="E6" s="8">
+        <v>60</v>
+      </c>
+      <c r="F6" s="8">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="8">
+        <v>189</v>
+      </c>
+      <c r="C7" s="8">
+        <v>150</v>
+      </c>
+      <c r="D7" s="8">
+        <v>85</v>
+      </c>
+      <c r="E7" s="8">
+        <v>192</v>
+      </c>
+      <c r="F7" s="8">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="8">
+        <v>189</v>
+      </c>
+      <c r="C8" s="8">
+        <v>150</v>
+      </c>
+      <c r="D8" s="8">
+        <v>85</v>
+      </c>
+      <c r="E8" s="8">
+        <v>192</v>
+      </c>
+      <c r="F8" s="8">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="8">
+        <v>20</v>
+      </c>
+      <c r="C9" s="8">
+        <v>75</v>
+      </c>
+      <c r="D9" s="8">
+        <v>56</v>
+      </c>
+      <c r="E9" s="8">
+        <v>27</v>
+      </c>
+      <c r="F9" s="8">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="8">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8">
+        <v>75</v>
+      </c>
+      <c r="D10" s="8">
+        <v>56</v>
+      </c>
+      <c r="E10" s="8">
+        <v>27</v>
+      </c>
+      <c r="F10" s="8">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="8">
+        <v>215</v>
+      </c>
+      <c r="C11" s="8">
+        <v>85</v>
+      </c>
+      <c r="D11" s="8">
+        <v>32</v>
+      </c>
+      <c r="E11" s="8">
+        <v>20</v>
+      </c>
+      <c r="F11" s="8">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="8">
+        <v>200</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="8">
+        <v>15</v>
+      </c>
+      <c r="C13" s="8">
+        <v>85</v>
+      </c>
+      <c r="D13" s="8">
+        <v>32</v>
+      </c>
+      <c r="E13" s="8">
+        <v>20</v>
+      </c>
+      <c r="F13" s="8">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8">
+        <v>155</v>
+      </c>
+      <c r="C14" s="8">
+        <v>85</v>
+      </c>
+      <c r="D14" s="8">
+        <v>155</v>
+      </c>
+      <c r="E14" s="8">
+        <v>155</v>
+      </c>
+      <c r="F14" s="8">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="8">
+        <v>155</v>
+      </c>
+      <c r="C15" s="8">
+        <v>85</v>
+      </c>
+      <c r="D15" s="8">
+        <v>155</v>
+      </c>
+      <c r="E15" s="8">
+        <v>155</v>
+      </c>
+      <c r="F15" s="8">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="8">
+        <v>408</v>
+      </c>
+      <c r="C16" s="8">
+        <v>476</v>
+      </c>
+      <c r="D16" s="8">
+        <v>305</v>
+      </c>
+      <c r="E16" s="8">
+        <v>353</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="8">
+        <v>56</v>
+      </c>
+      <c r="C17" s="8">
+        <v>85</v>
+      </c>
+      <c r="D17" s="8">
+        <v>3</v>
+      </c>
+      <c r="E17" s="8">
+        <v>45</v>
+      </c>
+      <c r="F17" s="8">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="8">
+        <v>31</v>
+      </c>
+      <c r="C18" s="8">
+        <v>135</v>
+      </c>
+      <c r="D18" s="8">
+        <v>75</v>
+      </c>
+      <c r="E18" s="8">
+        <v>76</v>
+      </c>
+      <c r="F18" s="8">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="8">
+        <v>80</v>
+      </c>
+      <c r="C19" s="8">
+        <v>74</v>
+      </c>
+      <c r="D19" s="8">
+        <v>65</v>
+      </c>
+      <c r="E19" s="8">
+        <v>89</v>
+      </c>
+      <c r="F19" s="8">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="8">
+        <v>132</v>
+      </c>
+      <c r="C20" s="8">
+        <v>145</v>
+      </c>
+      <c r="D20" s="8">
+        <v>73</v>
+      </c>
+      <c r="E20" s="8">
+        <v>46</v>
+      </c>
+      <c r="F20" s="8">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="8">
+        <v>17</v>
+      </c>
+      <c r="C21" s="8">
+        <v>8</v>
+      </c>
+      <c r="D21" s="8">
+        <v>35</v>
+      </c>
+      <c r="E21" s="8">
+        <v>28</v>
+      </c>
+      <c r="F21" s="8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="8">
+        <v>92</v>
+      </c>
+      <c r="C22" s="8">
+        <v>29</v>
+      </c>
+      <c r="D22" s="8">
+        <v>54</v>
+      </c>
+      <c r="E22" s="8">
+        <v>69</v>
+      </c>
+      <c r="F22" s="8">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1002</v>
+      </c>
+      <c r="C23" s="8">
+        <v>916</v>
+      </c>
+      <c r="D23" s="8">
+        <v>645</v>
+      </c>
+      <c r="E23" s="8">
+        <v>807</v>
+      </c>
+      <c r="F23" s="8">
+        <v>3370</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4882DA06-9C17-F241-8202-CBC2A88C4B8A}">
   <dimension ref="A1:H46"/>
   <sheetViews>

</xml_diff>